<commit_message>
Added background to readme, calculated throughput for 10 repl system
</commit_message>
<xml_diff>
--- a/docs/data10repl.xlsx
+++ b/docs/data10repl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USERDATA\chevrotain\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690529C5-26B2-4BC2-BD94-747F73519F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A225427-7B79-470F-AE06-0DED8B21CC04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A478AC17-B821-49E0-BBE5-2534ACF29465}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{A478AC17-B821-49E0-BBE5-2534ACF29465}"/>
   </bookViews>
   <sheets>
     <sheet name="CvRDT-Y" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
   <si>
     <t>10 ops/s</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Zero</t>
-  </si>
-  <si>
-    <t>Plus 5 zeros</t>
   </si>
   <si>
     <t>Consistently fails at 175ops/s</t>
@@ -142,11 +139,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1180,13 +1178,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AC6FEB-667F-4E3D-9C91-4638F2D64FB2}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17:L23"/>
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1949,12 +1950,121 @@
         <v>52.362768600000003</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N24" s="2">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>0</v>
+      </c>
+      <c r="R24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N25" s="2">
+        <v>0</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N27" s="2">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0</v>
+      </c>
+      <c r="P27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>0</v>
+      </c>
+      <c r="R27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <f>AVERAGE(N18:N27)</f>
+        <v>1998.4</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ref="O28:R28" si="3">AVERAGE(O18:O27)</f>
+        <v>999</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="3"/>
+        <v>899.5</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="3"/>
+        <v>499.6</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="3"/>
+        <v>499.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N30" s="4">
+        <f>O30/AVERAGE(N28:R28)</f>
+        <v>157577.61437908496</v>
+      </c>
+      <c r="O30" s="1">
+        <f>1543*100000</f>
+        <v>154300000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2202,7 +2312,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
@@ -2214,12 +2324,12 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N11" s="2"/>
     </row>
@@ -2279,9 +2389,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CE1395-6380-422A-83AF-3E7E185B3F85}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2315,6 +2431,14 @@
         <v>1708046</v>
       </c>
       <c r="O1" s="1"/>
+      <c r="P1">
+        <f>R1/B1</f>
+        <v>10.053435017019821</v>
+      </c>
+      <c r="R1" s="1">
+        <f>1543*100000</f>
+        <v>154300000</v>
+      </c>
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -2348,6 +2472,10 @@
       <c r="N2">
         <v>50</v>
       </c>
+      <c r="P2">
+        <f>R1/E1</f>
+        <v>24.954639322980473</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2380,6 +2508,10 @@
       <c r="N3">
         <v>49.164676999999998</v>
       </c>
+      <c r="P3">
+        <f>R1/H1</f>
+        <v>47.988181782840257</v>
+      </c>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2413,6 +2545,10 @@
       <c r="N4">
         <v>49.284004000000003</v>
       </c>
+      <c r="P4">
+        <f>R1/K1</f>
+        <v>71.56476379221823</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2445,6 +2581,10 @@
       <c r="N5">
         <v>49.642006000000002</v>
       </c>
+      <c r="P5">
+        <f>R1/N1</f>
+        <v>90.337145486714064</v>
+      </c>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2477,6 +2617,10 @@
       </c>
       <c r="N6">
         <v>49.284008</v>
+      </c>
+      <c r="P6">
+        <f>R1/B9</f>
+        <v>163.54694422657028</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -2521,8 +2665,17 @@
         <v>49.474938999999999</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="P7" s="2">
+        <f>R1/E9</f>
+        <v>192.5133156083009</v>
+      </c>
       <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f>R1/H9</f>
+        <v>334.88731465083168</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2556,6 +2709,10 @@
         <v>313804</v>
       </c>
       <c r="O9" s="1"/>
+      <c r="P9">
+        <f>R1/K9</f>
+        <v>467.69338954949274</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2588,6 +2745,10 @@
       <c r="N10">
         <v>52.505961999999997</v>
       </c>
+      <c r="P10">
+        <f>R1/N9</f>
+        <v>491.70820002294425</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2620,6 +2781,10 @@
       <c r="N11">
         <v>52.983294999999998</v>
       </c>
+      <c r="P11">
+        <f>R1/B17</f>
+        <v>882.26885470867398</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2652,6 +2817,10 @@
       <c r="N12">
         <v>52.744633</v>
       </c>
+      <c r="P12">
+        <f>R1/E17</f>
+        <v>892.37175409172403</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2683,6 +2852,10 @@
       </c>
       <c r="N13">
         <v>54.773269999999997</v>
+      </c>
+      <c r="P13">
+        <f>R1/H17</f>
+        <v>892.43885087653348</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2962,7 +3135,7 @@
         <v>51.455846600000008</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" ref="G23:L23" si="2">AVERAGE(G18:G22)</f>
+        <f t="shared" ref="G23:K23" si="2">AVERAGE(G18:G22)</f>
         <v>1998.40994</v>
       </c>
       <c r="H23" s="1">
@@ -2986,5 +3159,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>